<commit_message>
database : add eps data
</commit_message>
<xml_diff>
--- a/database/industries/bargh/bemoto/product/monthly.xlsx
+++ b/database/industries/bargh/bemoto/product/monthly.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trade\database\industries\bargh\bemoto\product\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Trade\database\industries\bargh\bemoto\product\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2126066E-1BDF-42D2-9222-92716574DA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="5550"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -258,7 +259,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -451,7 +452,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -463,7 +464,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -510,6 +511,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -545,6 +563,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -696,17 +731,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BB77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="54" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -761,7 +796,7 @@
       <c r="BA1" s="1"/>
       <c r="BB1" s="1"/>
     </row>
-    <row r="2" spans="2:54" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:54" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -818,7 +853,7 @@
       <c r="BA2" s="1"/>
       <c r="BB2" s="1"/>
     </row>
-    <row r="3" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -875,7 +910,7 @@
       <c r="BA3" s="1"/>
       <c r="BB3" s="1"/>
     </row>
-    <row r="4" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -930,7 +965,7 @@
       <c r="BA4" s="1"/>
       <c r="BB4" s="1"/>
     </row>
-    <row r="5" spans="2:54" ht="42" x14ac:dyDescent="0.65">
+    <row r="5" spans="2:54" ht="40.799999999999997" x14ac:dyDescent="0.75">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -987,7 +1022,7 @@
       <c r="BA5" s="4"/>
       <c r="BB5" s="4"/>
     </row>
-    <row r="6" spans="2:54" ht="42" x14ac:dyDescent="0.65">
+    <row r="6" spans="2:54" ht="40.799999999999997" x14ac:dyDescent="0.75">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1044,7 +1079,7 @@
       <c r="BA6" s="4"/>
       <c r="BB6" s="4"/>
     </row>
-    <row r="7" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1099,7 +1134,7 @@
       <c r="BA7" s="1"/>
       <c r="BB7" s="1"/>
     </row>
-    <row r="8" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:54" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -1256,7 +1291,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1311,7 +1346,7 @@
       <c r="BA9" s="1"/>
       <c r="BB9" s="1"/>
     </row>
-    <row r="10" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
         <v>4</v>
       </c>
@@ -1368,7 +1403,7 @@
       <c r="BA10" s="9"/>
       <c r="BB10" s="9"/>
     </row>
-    <row r="11" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
         <v>55</v>
       </c>
@@ -1527,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B12" s="12" t="s">
         <v>57</v>
       </c>
@@ -1686,7 +1721,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>59</v>
       </c>
@@ -1845,7 +1880,7 @@
         <v>56360</v>
       </c>
     </row>
-    <row r="14" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
         <v>60</v>
       </c>
@@ -2004,7 +2039,7 @@
         <v>10837</v>
       </c>
     </row>
-    <row r="15" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
         <v>61</v>
       </c>
@@ -2163,7 +2198,7 @@
         <v>79920</v>
       </c>
     </row>
-    <row r="16" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="s">
         <v>62</v>
       </c>
@@ -2322,7 +2357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B17" s="14" t="s">
         <v>63</v>
       </c>
@@ -2379,7 +2414,7 @@
       <c r="BA17" s="15"/>
       <c r="BB17" s="15"/>
     </row>
-    <row r="18" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B18" s="16" t="s">
         <v>64</v>
       </c>
@@ -2536,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
         <v>65</v>
       </c>
@@ -2693,7 +2728,7 @@
         <v>147117</v>
       </c>
     </row>
-    <row r="20" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2748,7 +2783,7 @@
       <c r="BA20" s="1"/>
       <c r="BB20" s="1"/>
     </row>
-    <row r="21" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2803,7 +2838,7 @@
       <c r="BA21" s="1"/>
       <c r="BB21" s="1"/>
     </row>
-    <row r="22" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2858,7 +2893,7 @@
       <c r="BA22" s="1"/>
       <c r="BB22" s="1"/>
     </row>
-    <row r="23" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:54" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
         <v>66</v>
       </c>
@@ -3015,7 +3050,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -3070,7 +3105,7 @@
       <c r="BA24" s="1"/>
       <c r="BB24" s="1"/>
     </row>
-    <row r="25" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="s">
         <v>66</v>
       </c>
@@ -3127,7 +3162,7 @@
       <c r="BA25" s="9"/>
       <c r="BB25" s="9"/>
     </row>
-    <row r="26" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B26" s="10" t="s">
         <v>55</v>
       </c>
@@ -3286,7 +3321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B27" s="12" t="s">
         <v>57</v>
       </c>
@@ -3445,7 +3480,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B28" s="10" t="s">
         <v>59</v>
       </c>
@@ -3604,7 +3639,7 @@
         <v>14800</v>
       </c>
     </row>
-    <row r="29" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B29" s="12" t="s">
         <v>60</v>
       </c>
@@ -3763,7 +3798,7 @@
         <v>16563</v>
       </c>
     </row>
-    <row r="30" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
         <v>61</v>
       </c>
@@ -3922,7 +3957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B31" s="12" t="s">
         <v>62</v>
       </c>
@@ -4081,7 +4116,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B32" s="14" t="s">
         <v>63</v>
       </c>
@@ -4138,7 +4173,7 @@
       <c r="BA32" s="15"/>
       <c r="BB32" s="15"/>
     </row>
-    <row r="33" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B33" s="16" t="s">
         <v>64</v>
       </c>
@@ -4295,7 +4330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B34" s="8" t="s">
         <v>67</v>
       </c>
@@ -4352,7 +4387,7 @@
       <c r="BA34" s="9"/>
       <c r="BB34" s="9"/>
     </row>
-    <row r="35" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B35" s="10" t="s">
         <v>55</v>
       </c>
@@ -4511,7 +4546,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B36" s="12" t="s">
         <v>59</v>
       </c>
@@ -4670,7 +4705,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B37" s="10" t="s">
         <v>60</v>
       </c>
@@ -4829,7 +4864,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B38" s="12" t="s">
         <v>61</v>
       </c>
@@ -4988,7 +5023,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B39" s="10" t="s">
         <v>62</v>
       </c>
@@ -5147,7 +5182,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B40" s="18" t="s">
         <v>68</v>
       </c>
@@ -5304,7 +5339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B41" s="16" t="s">
         <v>65</v>
       </c>
@@ -5461,7 +5496,7 @@
         <v>31437</v>
       </c>
     </row>
-    <row r="42" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -5516,7 +5551,7 @@
       <c r="BA42" s="1"/>
       <c r="BB42" s="1"/>
     </row>
-    <row r="43" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -5571,7 +5606,7 @@
       <c r="BA43" s="1"/>
       <c r="BB43" s="1"/>
     </row>
-    <row r="44" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -5626,7 +5661,7 @@
       <c r="BA44" s="1"/>
       <c r="BB44" s="1"/>
     </row>
-    <row r="45" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:54" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B45" s="7" t="s">
         <v>69</v>
       </c>
@@ -5783,7 +5818,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -5838,7 +5873,7 @@
       <c r="BA46" s="1"/>
       <c r="BB46" s="1"/>
     </row>
-    <row r="47" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B47" s="8" t="s">
         <v>69</v>
       </c>
@@ -5895,7 +5930,7 @@
       <c r="BA47" s="9"/>
       <c r="BB47" s="9"/>
     </row>
-    <row r="48" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B48" s="10" t="s">
         <v>55</v>
       </c>
@@ -6054,7 +6089,7 @@
         <v>27550</v>
       </c>
     </row>
-    <row r="49" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B49" s="12" t="s">
         <v>57</v>
       </c>
@@ -6213,7 +6248,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B50" s="10" t="s">
         <v>59</v>
       </c>
@@ -6372,7 +6407,7 @@
         <v>220719</v>
       </c>
     </row>
-    <row r="51" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B51" s="12" t="s">
         <v>60</v>
       </c>
@@ -6531,7 +6566,7 @@
         <v>780408</v>
       </c>
     </row>
-    <row r="52" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B52" s="10" t="s">
         <v>61</v>
       </c>
@@ -6690,7 +6725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B53" s="12" t="s">
         <v>62</v>
       </c>
@@ -6849,7 +6884,7 @@
         <v>10636</v>
       </c>
     </row>
-    <row r="54" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B54" s="14" t="s">
         <v>71</v>
       </c>
@@ -6906,7 +6941,7 @@
       <c r="BA54" s="15"/>
       <c r="BB54" s="15"/>
     </row>
-    <row r="55" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B55" s="16" t="s">
         <v>64</v>
       </c>
@@ -7065,7 +7100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B56" s="8" t="s">
         <v>72</v>
       </c>
@@ -7122,7 +7157,7 @@
       <c r="BA56" s="9"/>
       <c r="BB56" s="9"/>
     </row>
-    <row r="57" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B57" s="10" t="s">
         <v>55</v>
       </c>
@@ -7281,7 +7316,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B58" s="12" t="s">
         <v>59</v>
       </c>
@@ -7440,7 +7475,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B59" s="10" t="s">
         <v>60</v>
       </c>
@@ -7599,7 +7634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B60" s="12" t="s">
         <v>61</v>
       </c>
@@ -7758,7 +7793,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B61" s="10" t="s">
         <v>62</v>
       </c>
@@ -7917,7 +7952,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B62" s="18" t="s">
         <v>68</v>
       </c>
@@ -8076,7 +8111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B63" s="8" t="s">
         <v>73</v>
       </c>
@@ -8133,7 +8168,7 @@
       <c r="BA63" s="9"/>
       <c r="BB63" s="9"/>
     </row>
-    <row r="64" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B64" s="10" t="s">
         <v>74</v>
       </c>
@@ -8292,7 +8327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B65" s="18" t="s">
         <v>65</v>
       </c>
@@ -8449,7 +8484,7 @@
         <v>1039313</v>
       </c>
     </row>
-    <row r="66" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -8504,7 +8539,7 @@
       <c r="BA66" s="1"/>
       <c r="BB66" s="1"/>
     </row>
-    <row r="67" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -8559,7 +8594,7 @@
       <c r="BA67" s="1"/>
       <c r="BB67" s="1"/>
     </row>
-    <row r="68" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -8614,7 +8649,7 @@
       <c r="BA68" s="1"/>
       <c r="BB68" s="1"/>
     </row>
-    <row r="69" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:54" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B69" s="7" t="s">
         <v>75</v>
       </c>
@@ -8771,7 +8806,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -8826,7 +8861,7 @@
       <c r="BA70" s="1"/>
       <c r="BB70" s="1"/>
     </row>
-    <row r="71" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B71" s="8" t="s">
         <v>76</v>
       </c>
@@ -8883,7 +8918,7 @@
       <c r="BA71" s="9"/>
       <c r="BB71" s="9"/>
     </row>
-    <row r="72" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B72" s="10" t="s">
         <v>55</v>
       </c>
@@ -9042,7 +9077,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B73" s="12" t="s">
         <v>57</v>
       </c>
@@ -9201,7 +9236,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B74" s="10" t="s">
         <v>59</v>
       </c>
@@ -9360,7 +9395,7 @@
         <v>14913446</v>
       </c>
     </row>
-    <row r="75" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B75" s="12" t="s">
         <v>60</v>
       </c>
@@ -9519,7 +9554,7 @@
         <v>47117551</v>
       </c>
     </row>
-    <row r="76" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B76" s="10" t="s">
         <v>61</v>
       </c>
@@ -9678,7 +9713,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="77" spans="2:54" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:54" x14ac:dyDescent="0.3">
       <c r="B77" s="12" t="s">
         <v>62</v>
       </c>

</xml_diff>